<commit_message>
"Swagger to Excel modified"
</commit_message>
<xml_diff>
--- a/testData/practice.xlsx
+++ b/testData/practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\3D Objects\automation framework\RestAssuredAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C712E48-50C9-4CEB-8DCA-E6F2B43357A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775DE6F6-55BE-46F7-8C2B-61986A44FAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t/>
   </si>
@@ -79,7 +79,7 @@
     <t>Create Job</t>
   </si>
   <si>
-    <t>Delete User Parameter</t>
+    <t>testDeleteUserParameter</t>
   </si>
   <si>
     <t>The user email</t>
@@ -88,16 +88,16 @@
     <t>Enter value</t>
   </si>
   <si>
-    <t>Get Single Job Parameter</t>
+    <t>testGetSingleJobParameter</t>
   </si>
   <si>
     <t>The job ID</t>
   </si>
   <si>
-    <t>Update Job Parameter</t>
-  </si>
-  <si>
-    <t>Delete Job Parameter</t>
+    <t>testUpdateJobParameter</t>
+  </si>
+  <si>
+    <t>testDeleteJobParameter</t>
   </si>
   <si>
     <t>testUpdateJob</t>
@@ -184,7 +184,7 @@
     <t>job.position</t>
   </si>
   <si>
-    <t>job.status</t>
+    <t xml:space="preserve">job.status </t>
   </si>
   <si>
     <t>jobs[0].company</t>
@@ -194,15 +194,6 @@
   </si>
   <si>
     <t>jobs[0].status</t>
-  </si>
-  <si>
-    <t>accops</t>
-  </si>
-  <si>
-    <t>shrikant</t>
-  </si>
-  <si>
-    <t>shrikant@accops.in</t>
   </si>
 </sst>
 </file>
@@ -577,17 +568,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -781,7 +772,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -899,88 +890,80 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>0</v>
-      </c>
+      <c r="B50" s="3"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -989,103 +972,106 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>57</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>43</v>
-      </c>
-      <c r="B72" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>0</v>
-      </c>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B77" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1093,11 +1079,15 @@
         <v>0</v>
       </c>
     </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B49" r:id="rId1" xr:uid="{59521F86-C3F4-43B3-AF72-3FBEEB765C4F}"/>
-    <hyperlink ref="A18" r:id="rId2" xr:uid="{F93490BD-212B-4C8B-8848-50640BBD70B7}"/>
-    <hyperlink ref="C61" r:id="rId3" xr:uid="{18FBDF17-0100-43F3-8A13-CC60037801CC}"/>
+    <hyperlink ref="B49" r:id="rId1" xr:uid="{79C38744-701B-49B1-8070-A2B6F73BC495}"/>
+    <hyperlink ref="A18" r:id="rId2" xr:uid="{77DC3961-02B4-4E81-A49C-2E6DA9EA4577}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>